<commit_message>
make sql create table
</commit_message>
<xml_diff>
--- a/共同研修課題_設計メモ_2024-12-09_栗原.xlsx
+++ b/共同研修課題_設計メモ_2024-12-09_栗原.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\しぶや\Desktop\VB課題資料\課題３(共同)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\しぶや\Desktop\ProjectC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C2C86A-FFF4-4B78-936E-421EB7057116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DE7799-37AA-4E11-84BB-C094C227B7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="課題5" sheetId="5" r:id="rId1"/>
@@ -5196,7 +5196,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5519,11 +5519,32 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -5540,25 +5561,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -7447,8 +7457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E20C55-54EF-495E-B2C0-1D67D38AE4AA}">
   <dimension ref="B2:P84"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -7501,18 +7511,18 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B4" s="77"/>
-      <c r="C4" s="116" t="s">
+      <c r="C4" s="123" t="s">
         <v>291</v>
       </c>
-      <c r="D4" s="117"/>
-      <c r="E4" s="118" t="s">
+      <c r="D4" s="124"/>
+      <c r="E4" s="125" t="s">
         <v>243</v>
       </c>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="120"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="126"/>
+      <c r="H4" s="126"/>
+      <c r="I4" s="126"/>
+      <c r="J4" s="127"/>
       <c r="K4" s="71"/>
       <c r="L4" s="71"/>
       <c r="M4" s="78"/>
@@ -7520,18 +7530,18 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B5" s="77"/>
-      <c r="C5" s="116" t="s">
+      <c r="C5" s="123" t="s">
         <v>292</v>
       </c>
-      <c r="D5" s="117"/>
-      <c r="E5" s="118" t="s">
+      <c r="D5" s="124"/>
+      <c r="E5" s="125" t="s">
         <v>321</v>
       </c>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="120"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="J5" s="127"/>
       <c r="K5" s="71"/>
       <c r="L5" s="71"/>
       <c r="M5" s="78"/>
@@ -7556,19 +7566,19 @@
       <c r="C7" s="121" t="s">
         <v>293</v>
       </c>
-      <c r="D7" s="123" t="s">
+      <c r="D7" s="128" t="s">
         <v>294</v>
       </c>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123" t="s">
+      <c r="E7" s="128"/>
+      <c r="F7" s="128" t="s">
         <v>295</v>
       </c>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123" t="s">
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="128" t="s">
         <v>296</v>
       </c>
-      <c r="J7" s="123"/>
+      <c r="J7" s="128"/>
       <c r="K7" s="121" t="s">
         <v>297</v>
       </c>
@@ -8008,8 +8018,8 @@
       <c r="L24" s="85"/>
       <c r="M24" s="87"/>
     </row>
-    <row r="25" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="2:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:13" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="73"/>
       <c r="C26" s="74"/>
       <c r="D26" s="74"/>
@@ -8025,36 +8035,36 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B27" s="77"/>
-      <c r="C27" s="116" t="s">
+      <c r="C27" s="123" t="s">
         <v>291</v>
       </c>
-      <c r="D27" s="117"/>
-      <c r="E27" s="118" t="s">
-        <v>265</v>
-      </c>
-      <c r="F27" s="119"/>
-      <c r="G27" s="119"/>
-      <c r="H27" s="119"/>
-      <c r="I27" s="119"/>
-      <c r="J27" s="120"/>
+      <c r="D27" s="124"/>
+      <c r="E27" s="125" t="s">
+        <v>267</v>
+      </c>
+      <c r="F27" s="126"/>
+      <c r="G27" s="126"/>
+      <c r="H27" s="126"/>
+      <c r="I27" s="126"/>
+      <c r="J27" s="127"/>
       <c r="K27" s="71"/>
       <c r="L27" s="71"/>
       <c r="M27" s="78"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B28" s="77"/>
-      <c r="C28" s="116" t="s">
+      <c r="C28" s="123" t="s">
         <v>292</v>
       </c>
-      <c r="D28" s="117"/>
-      <c r="E28" s="118" t="s">
-        <v>353</v>
-      </c>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="119"/>
-      <c r="I28" s="119"/>
-      <c r="J28" s="120"/>
+      <c r="D28" s="124"/>
+      <c r="E28" s="125" t="s">
+        <v>365</v>
+      </c>
+      <c r="F28" s="126"/>
+      <c r="G28" s="126"/>
+      <c r="H28" s="126"/>
+      <c r="I28" s="126"/>
+      <c r="J28" s="127"/>
       <c r="K28" s="71"/>
       <c r="L28" s="71"/>
       <c r="M28" s="78"/>
@@ -8078,19 +8088,19 @@
       <c r="C30" s="121" t="s">
         <v>293</v>
       </c>
-      <c r="D30" s="123" t="s">
+      <c r="D30" s="128" t="s">
         <v>294</v>
       </c>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123" t="s">
+      <c r="E30" s="128"/>
+      <c r="F30" s="128" t="s">
         <v>295</v>
       </c>
-      <c r="G30" s="123"/>
-      <c r="H30" s="123"/>
-      <c r="I30" s="123" t="s">
+      <c r="G30" s="128"/>
+      <c r="H30" s="128"/>
+      <c r="I30" s="128" t="s">
         <v>296</v>
       </c>
-      <c r="J30" s="123"/>
+      <c r="J30" s="128"/>
       <c r="K30" s="121" t="s">
         <v>297</v>
       </c>
@@ -8132,1041 +8142,1070 @@
       <c r="C32" s="80">
         <v>1</v>
       </c>
-      <c r="D32" s="81" t="s">
-        <v>264</v>
+      <c r="D32" s="18" t="s">
+        <v>268</v>
       </c>
       <c r="E32" s="88" t="s">
-        <v>345</v>
-      </c>
-      <c r="F32" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="G32" s="79"/>
-      <c r="H32" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="I32" s="88" t="s">
-        <v>333</v>
-      </c>
-      <c r="J32" s="79"/>
+        <v>346</v>
+      </c>
+      <c r="F32" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="H32" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="I32" s="81" t="s">
+        <v>340</v>
+      </c>
+      <c r="J32" s="79">
+        <v>3</v>
+      </c>
       <c r="K32" s="81"/>
-      <c r="L32" s="89" t="s">
-        <v>350</v>
+      <c r="L32" s="81" t="s">
+        <v>351</v>
       </c>
       <c r="M32" s="78"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B33" s="77"/>
       <c r="C33" s="80">
         <v>2</v>
       </c>
-      <c r="D33" s="81" t="s">
-        <v>282</v>
-      </c>
-      <c r="E33" s="81" t="s">
-        <v>342</v>
+      <c r="D33" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="E33" s="88" t="s">
+        <v>364</v>
       </c>
       <c r="F33" s="79"/>
       <c r="G33" s="79"/>
-      <c r="H33" s="38" t="s">
-        <v>332</v>
+      <c r="H33" s="79" t="s">
+        <v>331</v>
       </c>
       <c r="I33" s="88" t="s">
-        <v>307</v>
-      </c>
-      <c r="J33" s="79"/>
+        <v>335</v>
+      </c>
+      <c r="J33" s="79">
+        <v>10</v>
+      </c>
       <c r="K33" s="81"/>
       <c r="L33" s="81"/>
       <c r="M33" s="78"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B34" s="77"/>
       <c r="C34" s="80">
         <v>3</v>
       </c>
-      <c r="D34" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="88" t="s">
-        <v>318</v>
-      </c>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
       <c r="F34" s="79"/>
-      <c r="G34" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="H34" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="I34" s="88" t="s">
-        <v>306</v>
-      </c>
-      <c r="J34" s="79">
-        <v>5</v>
-      </c>
+      <c r="G34" s="79"/>
+      <c r="H34" s="79"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="79"/>
       <c r="K34" s="81"/>
-      <c r="L34" s="88" t="s">
-        <v>352</v>
-      </c>
+      <c r="L34" s="81"/>
       <c r="M34" s="78"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B35" s="77"/>
       <c r="C35" s="80">
         <v>4</v>
       </c>
-      <c r="D35" s="88" t="s">
-        <v>262</v>
-      </c>
-      <c r="E35" s="88" t="s">
-        <v>356</v>
-      </c>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
       <c r="F35" s="79"/>
-      <c r="G35" s="38" t="s">
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="81"/>
+      <c r="M35" s="78"/>
+    </row>
+    <row r="36" spans="2:13" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B36" s="84"/>
+      <c r="C36" s="85"/>
+      <c r="D36" s="85"/>
+      <c r="E36" s="85"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="85"/>
+      <c r="J36" s="86"/>
+      <c r="K36" s="85"/>
+      <c r="L36" s="85"/>
+      <c r="M36" s="87"/>
+    </row>
+    <row r="37" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="38" spans="2:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="73"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="74"/>
+      <c r="M38" s="76"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B39" s="77"/>
+      <c r="C39" s="123" t="s">
+        <v>291</v>
+      </c>
+      <c r="D39" s="124"/>
+      <c r="E39" s="125" t="s">
+        <v>250</v>
+      </c>
+      <c r="F39" s="126"/>
+      <c r="G39" s="126"/>
+      <c r="H39" s="126"/>
+      <c r="I39" s="126"/>
+      <c r="J39" s="127"/>
+      <c r="K39" s="129"/>
+      <c r="L39" s="129"/>
+      <c r="M39" s="78"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B40" s="77"/>
+      <c r="C40" s="123" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" s="124"/>
+      <c r="E40" s="125" t="s">
+        <v>963</v>
+      </c>
+      <c r="F40" s="126"/>
+      <c r="G40" s="126"/>
+      <c r="H40" s="126"/>
+      <c r="I40" s="126"/>
+      <c r="J40" s="127"/>
+      <c r="K40" s="129"/>
+      <c r="L40" s="129"/>
+      <c r="M40" s="78"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B41" s="77"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="129"/>
+      <c r="E41" s="129"/>
+      <c r="F41" s="129"/>
+      <c r="G41" s="129"/>
+      <c r="H41" s="129"/>
+      <c r="I41" s="129"/>
+      <c r="J41" s="130"/>
+      <c r="K41" s="129"/>
+      <c r="L41" s="129"/>
+      <c r="M41" s="78"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B42" s="77"/>
+      <c r="C42" s="121" t="s">
+        <v>293</v>
+      </c>
+      <c r="D42" s="128" t="s">
+        <v>294</v>
+      </c>
+      <c r="E42" s="128"/>
+      <c r="F42" s="128" t="s">
+        <v>295</v>
+      </c>
+      <c r="G42" s="128"/>
+      <c r="H42" s="128"/>
+      <c r="I42" s="128" t="s">
+        <v>296</v>
+      </c>
+      <c r="J42" s="128"/>
+      <c r="K42" s="121" t="s">
+        <v>297</v>
+      </c>
+      <c r="L42" s="121" t="s">
+        <v>298</v>
+      </c>
+      <c r="M42" s="78"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B43" s="77"/>
+      <c r="C43" s="122"/>
+      <c r="D43" s="114" t="s">
+        <v>299</v>
+      </c>
+      <c r="E43" s="114" t="s">
+        <v>300</v>
+      </c>
+      <c r="F43" s="114" t="s">
+        <v>301</v>
+      </c>
+      <c r="G43" s="114" t="s">
+        <v>302</v>
+      </c>
+      <c r="H43" s="114" t="s">
+        <v>303</v>
+      </c>
+      <c r="I43" s="114" t="s">
+        <v>304</v>
+      </c>
+      <c r="J43" s="114" t="s">
+        <v>305</v>
+      </c>
+      <c r="K43" s="122"/>
+      <c r="L43" s="122"/>
+      <c r="M43" s="78"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B44" s="77"/>
+      <c r="C44" s="80">
+        <v>1</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>959</v>
+      </c>
+      <c r="E44" s="88" t="s">
+        <v>964</v>
+      </c>
+      <c r="F44" s="38" t="s">
         <v>332</v>
       </c>
-      <c r="H35" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="I35" s="88" t="s">
-        <v>306</v>
-      </c>
-      <c r="J35" s="79">
-        <v>5</v>
-      </c>
-      <c r="K35" s="81"/>
-      <c r="L35" s="88" t="s">
-        <v>363</v>
-      </c>
-      <c r="M35" s="78"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B36" s="77"/>
-      <c r="C36" s="80">
-        <v>5</v>
-      </c>
-      <c r="D36" s="88" t="s">
-        <v>309</v>
-      </c>
-      <c r="E36" s="81" t="s">
-        <v>343</v>
-      </c>
-      <c r="F36" s="79"/>
-      <c r="H36" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="I36" s="88" t="s">
-        <v>333</v>
-      </c>
-      <c r="J36" s="79"/>
-      <c r="K36" s="81"/>
-      <c r="L36" s="81"/>
-      <c r="M36" s="78"/>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B37" s="77"/>
-      <c r="C37" s="80">
-        <v>6</v>
-      </c>
-      <c r="D37" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37" s="81" t="s">
-        <v>344</v>
-      </c>
-      <c r="F37" s="79"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="I37" s="88" t="s">
-        <v>333</v>
-      </c>
-      <c r="J37" s="79"/>
-      <c r="K37" s="81"/>
-      <c r="L37" s="81"/>
-      <c r="M37" s="78"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B38" s="77"/>
-      <c r="C38" s="80">
-        <v>7</v>
-      </c>
-      <c r="D38" s="81" t="s">
-        <v>268</v>
-      </c>
-      <c r="E38" s="88" t="s">
-        <v>346</v>
-      </c>
-      <c r="F38" s="79"/>
-      <c r="G38" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="H38" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="I38" s="88" t="s">
-        <v>306</v>
-      </c>
-      <c r="J38" s="79">
+      <c r="G44" s="131"/>
+      <c r="H44" s="114" t="s">
+        <v>331</v>
+      </c>
+      <c r="I44" s="81" t="s">
+        <v>340</v>
+      </c>
+      <c r="J44" s="114">
+        <v>2</v>
+      </c>
+      <c r="K44" s="81"/>
+      <c r="L44" s="81" t="s">
+        <v>362</v>
+      </c>
+      <c r="M44" s="78"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B45" s="77"/>
+      <c r="C45" s="80">
+        <v>2</v>
+      </c>
+      <c r="D45" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="88" t="s">
+        <v>357</v>
+      </c>
+      <c r="F45" s="114"/>
+      <c r="G45" s="114"/>
+      <c r="H45" s="114" t="s">
+        <v>331</v>
+      </c>
+      <c r="I45" s="88" t="s">
+        <v>962</v>
+      </c>
+      <c r="J45" s="114">
+        <v>10</v>
+      </c>
+      <c r="K45" s="81"/>
+      <c r="L45" s="81"/>
+      <c r="M45" s="78"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B46" s="77"/>
+      <c r="C46" s="80">
         <v>3</v>
       </c>
-      <c r="K38" s="81"/>
-      <c r="L38" s="88" t="s">
-        <v>351</v>
-      </c>
-      <c r="M38" s="78"/>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B39" s="77"/>
-      <c r="C39" s="80">
-        <v>8</v>
-      </c>
-      <c r="D39" s="88"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="81"/>
-      <c r="L39" s="82"/>
-      <c r="M39" s="78"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B40" s="77"/>
-      <c r="C40" s="80">
-        <v>9</v>
-      </c>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="79"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="79"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="83"/>
-      <c r="M40" s="78"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B41" s="77"/>
-      <c r="C41" s="80">
-        <v>10</v>
-      </c>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="79"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="81"/>
-      <c r="J41" s="79"/>
-      <c r="K41" s="81"/>
-      <c r="L41" s="81"/>
-      <c r="M41" s="78"/>
-    </row>
-    <row r="42" spans="2:14" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B42" s="84"/>
-      <c r="C42" s="85"/>
-      <c r="D42" s="85"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="85"/>
-      <c r="G42" s="85"/>
-      <c r="H42" s="85"/>
-      <c r="I42" s="85"/>
-      <c r="J42" s="86"/>
-      <c r="K42" s="85"/>
-      <c r="L42" s="85"/>
-      <c r="M42" s="87"/>
-    </row>
-    <row r="43" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="44" spans="2:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="73"/>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="74"/>
-      <c r="I44" s="74"/>
-      <c r="J44" s="75"/>
-      <c r="K44" s="74"/>
-      <c r="L44" s="74"/>
-      <c r="M44" s="76"/>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B45" s="77"/>
-      <c r="C45" s="116" t="s">
-        <v>291</v>
-      </c>
-      <c r="D45" s="117"/>
-      <c r="E45" s="118" t="s">
-        <v>244</v>
-      </c>
-      <c r="F45" s="119"/>
-      <c r="G45" s="119"/>
-      <c r="H45" s="119"/>
-      <c r="I45" s="119"/>
-      <c r="J45" s="120"/>
-      <c r="K45" s="71"/>
-      <c r="L45" s="71"/>
-      <c r="M45" s="78"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B46" s="77"/>
-      <c r="C46" s="116" t="s">
-        <v>292</v>
-      </c>
-      <c r="D46" s="117"/>
-      <c r="E46" s="118" t="s">
-        <v>354</v>
-      </c>
-      <c r="F46" s="119"/>
-      <c r="G46" s="119"/>
-      <c r="H46" s="119"/>
-      <c r="I46" s="119"/>
-      <c r="J46" s="120"/>
-      <c r="K46" s="71"/>
-      <c r="L46" s="71"/>
+      <c r="D46" s="81"/>
+      <c r="E46" s="81"/>
+      <c r="F46" s="114"/>
+      <c r="G46" s="114"/>
+      <c r="H46" s="114"/>
+      <c r="I46" s="81"/>
+      <c r="J46" s="114"/>
+      <c r="K46" s="81"/>
+      <c r="L46" s="81"/>
       <c r="M46" s="78"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B47" s="77"/>
-      <c r="C47" s="71"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="71"/>
-      <c r="L47" s="71"/>
+      <c r="C47" s="80">
+        <v>4</v>
+      </c>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="114"/>
+      <c r="G47" s="114"/>
+      <c r="H47" s="114"/>
+      <c r="I47" s="81"/>
+      <c r="J47" s="114"/>
+      <c r="K47" s="81"/>
+      <c r="L47" s="81"/>
       <c r="M47" s="78"/>
-      <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B48" s="77"/>
-      <c r="C48" s="121" t="s">
-        <v>293</v>
-      </c>
-      <c r="D48" s="123" t="s">
-        <v>294</v>
-      </c>
-      <c r="E48" s="123"/>
-      <c r="F48" s="123" t="s">
-        <v>295</v>
-      </c>
-      <c r="G48" s="123"/>
-      <c r="H48" s="123"/>
-      <c r="I48" s="123" t="s">
-        <v>296</v>
-      </c>
-      <c r="J48" s="123"/>
-      <c r="K48" s="121" t="s">
-        <v>297</v>
-      </c>
-      <c r="L48" s="121" t="s">
-        <v>298</v>
-      </c>
-      <c r="M48" s="78"/>
-      <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B49" s="77"/>
-      <c r="C49" s="122"/>
-      <c r="D49" s="79" t="s">
-        <v>299</v>
-      </c>
-      <c r="E49" s="79" t="s">
-        <v>300</v>
-      </c>
-      <c r="F49" s="79" t="s">
-        <v>301</v>
-      </c>
-      <c r="G49" s="79" t="s">
-        <v>302</v>
-      </c>
-      <c r="H49" s="79" t="s">
-        <v>303</v>
-      </c>
-      <c r="I49" s="79" t="s">
-        <v>304</v>
-      </c>
-      <c r="J49" s="79" t="s">
-        <v>305</v>
-      </c>
-      <c r="K49" s="122"/>
-      <c r="L49" s="122"/>
-      <c r="M49" s="78"/>
-      <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B50" s="77"/>
-      <c r="C50" s="80">
-        <v>1</v>
-      </c>
-      <c r="D50" s="81" t="s">
-        <v>262</v>
-      </c>
-      <c r="E50" s="81" t="s">
-        <v>355</v>
-      </c>
-      <c r="F50" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="G50" s="79"/>
-      <c r="H50" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I50" s="81" t="s">
-        <v>340</v>
-      </c>
-      <c r="J50" s="79">
-        <v>5</v>
-      </c>
-      <c r="K50" s="81"/>
-      <c r="L50" s="88" t="s">
-        <v>363</v>
-      </c>
-      <c r="M50" s="78"/>
-      <c r="N50" s="1"/>
+    </row>
+    <row r="48" spans="2:13" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="84"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="85"/>
+      <c r="F48" s="85"/>
+      <c r="G48" s="85"/>
+      <c r="H48" s="85"/>
+      <c r="I48" s="85"/>
+      <c r="J48" s="86"/>
+      <c r="K48" s="85"/>
+      <c r="L48" s="85"/>
+      <c r="M48" s="87"/>
+    </row>
+    <row r="49" spans="2:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="129"/>
+      <c r="C49" s="129"/>
+      <c r="D49" s="129"/>
+      <c r="E49" s="129"/>
+      <c r="F49" s="129"/>
+      <c r="G49" s="129"/>
+      <c r="H49" s="129"/>
+      <c r="I49" s="129"/>
+      <c r="J49" s="130"/>
+      <c r="K49" s="129"/>
+      <c r="L49" s="129"/>
+      <c r="M49" s="129"/>
+    </row>
+    <row r="50" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B50" s="73"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="75"/>
+      <c r="K50" s="74"/>
+      <c r="L50" s="74"/>
+      <c r="M50" s="76"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B51" s="77"/>
-      <c r="C51" s="80">
-        <v>2</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>959</v>
-      </c>
-      <c r="E51" s="88" t="s">
-        <v>964</v>
-      </c>
-      <c r="F51" s="79"/>
-      <c r="G51" s="111" t="s">
-        <v>331</v>
-      </c>
-      <c r="H51" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I51" s="88" t="s">
-        <v>306</v>
-      </c>
-      <c r="J51" s="79">
-        <v>2</v>
-      </c>
-      <c r="K51" s="81"/>
-      <c r="L51" s="88" t="s">
-        <v>362</v>
-      </c>
+      <c r="C51" s="123" t="s">
+        <v>291</v>
+      </c>
+      <c r="D51" s="124"/>
+      <c r="E51" s="125" t="s">
+        <v>244</v>
+      </c>
+      <c r="F51" s="126"/>
+      <c r="G51" s="126"/>
+      <c r="H51" s="126"/>
+      <c r="I51" s="126"/>
+      <c r="J51" s="127"/>
+      <c r="K51" s="71"/>
+      <c r="L51" s="71"/>
       <c r="M51" s="78"/>
-      <c r="N51" s="1"/>
-      <c r="P51" s="3"/>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B52" s="77"/>
-      <c r="C52" s="80">
-        <v>3</v>
-      </c>
-      <c r="D52" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="E52" s="81" t="s">
-        <v>358</v>
-      </c>
-      <c r="F52" s="79"/>
-      <c r="G52" s="79"/>
-      <c r="H52" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I52" s="88" t="s">
-        <v>962</v>
-      </c>
-      <c r="J52" s="79">
-        <v>10</v>
-      </c>
-      <c r="K52" s="81"/>
-      <c r="L52" s="81"/>
+      <c r="C52" s="123" t="s">
+        <v>292</v>
+      </c>
+      <c r="D52" s="124"/>
+      <c r="E52" s="125" t="s">
+        <v>354</v>
+      </c>
+      <c r="F52" s="126"/>
+      <c r="G52" s="126"/>
+      <c r="H52" s="126"/>
+      <c r="I52" s="126"/>
+      <c r="J52" s="127"/>
+      <c r="K52" s="71"/>
+      <c r="L52" s="71"/>
       <c r="M52" s="78"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B53" s="77"/>
-      <c r="C53" s="80">
-        <v>4</v>
-      </c>
-      <c r="D53" s="81" t="s">
-        <v>69</v>
-      </c>
-      <c r="E53" s="81" t="s">
-        <v>359</v>
-      </c>
-      <c r="F53" s="79"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I53" s="88" t="s">
-        <v>962</v>
-      </c>
-      <c r="J53" s="79">
-        <v>10</v>
-      </c>
-      <c r="K53" s="81"/>
-      <c r="L53" s="81"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
+      <c r="I53" s="71"/>
+      <c r="J53" s="72"/>
+      <c r="K53" s="71"/>
+      <c r="L53" s="71"/>
       <c r="M53" s="78"/>
+      <c r="N53" s="1"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B54" s="77"/>
-      <c r="C54" s="80">
-        <v>5</v>
-      </c>
-      <c r="D54" s="81" t="s">
-        <v>70</v>
-      </c>
-      <c r="E54" s="81" t="s">
-        <v>343</v>
-      </c>
-      <c r="F54" s="79"/>
-      <c r="G54" s="79"/>
-      <c r="H54" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I54" s="88" t="s">
-        <v>965</v>
-      </c>
-      <c r="J54" s="79"/>
-      <c r="K54" s="81"/>
-      <c r="L54" s="81"/>
+      <c r="C54" s="121" t="s">
+        <v>293</v>
+      </c>
+      <c r="D54" s="128" t="s">
+        <v>294</v>
+      </c>
+      <c r="E54" s="128"/>
+      <c r="F54" s="128" t="s">
+        <v>295</v>
+      </c>
+      <c r="G54" s="128"/>
+      <c r="H54" s="128"/>
+      <c r="I54" s="128" t="s">
+        <v>296</v>
+      </c>
+      <c r="J54" s="128"/>
+      <c r="K54" s="121" t="s">
+        <v>297</v>
+      </c>
+      <c r="L54" s="121" t="s">
+        <v>298</v>
+      </c>
       <c r="M54" s="78"/>
+      <c r="N54" s="1"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B55" s="77"/>
-      <c r="C55" s="80">
-        <v>6</v>
-      </c>
-      <c r="D55" s="81" t="s">
-        <v>360</v>
-      </c>
-      <c r="E55" s="81" t="s">
-        <v>361</v>
-      </c>
-      <c r="F55" s="79"/>
-      <c r="G55" s="79"/>
+      <c r="C55" s="122"/>
+      <c r="D55" s="79" t="s">
+        <v>299</v>
+      </c>
+      <c r="E55" s="79" t="s">
+        <v>300</v>
+      </c>
+      <c r="F55" s="79" t="s">
+        <v>301</v>
+      </c>
+      <c r="G55" s="79" t="s">
+        <v>302</v>
+      </c>
       <c r="H55" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I55" s="88" t="s">
-        <v>965</v>
-      </c>
-      <c r="J55" s="79"/>
-      <c r="K55" s="81"/>
-      <c r="L55" s="81"/>
+        <v>303</v>
+      </c>
+      <c r="I55" s="79" t="s">
+        <v>304</v>
+      </c>
+      <c r="J55" s="79" t="s">
+        <v>305</v>
+      </c>
+      <c r="K55" s="122"/>
+      <c r="L55" s="122"/>
       <c r="M55" s="78"/>
+      <c r="N55" s="1"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B56" s="77"/>
       <c r="C56" s="80">
-        <v>7</v>
-      </c>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="79"/>
+        <v>1</v>
+      </c>
+      <c r="D56" s="81" t="s">
+        <v>262</v>
+      </c>
+      <c r="E56" s="81" t="s">
+        <v>355</v>
+      </c>
+      <c r="F56" s="79" t="s">
+        <v>331</v>
+      </c>
       <c r="G56" s="79"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="88"/>
-      <c r="J56" s="79"/>
+      <c r="H56" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="I56" s="81" t="s">
+        <v>340</v>
+      </c>
+      <c r="J56" s="79">
+        <v>5</v>
+      </c>
       <c r="K56" s="81"/>
-      <c r="L56" s="81"/>
+      <c r="L56" s="88" t="s">
+        <v>363</v>
+      </c>
       <c r="M56" s="78"/>
+      <c r="N56" s="1"/>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B57" s="77"/>
       <c r="C57" s="80">
-        <v>8</v>
-      </c>
-      <c r="D57" s="81"/>
-      <c r="E57" s="81"/>
+        <v>2</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>959</v>
+      </c>
+      <c r="E57" s="88" t="s">
+        <v>964</v>
+      </c>
       <c r="F57" s="79"/>
-      <c r="G57" s="79"/>
-      <c r="H57" s="79"/>
-      <c r="I57" s="81"/>
-      <c r="J57" s="79"/>
+      <c r="G57" s="111" t="s">
+        <v>331</v>
+      </c>
+      <c r="H57" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="I57" s="88" t="s">
+        <v>306</v>
+      </c>
+      <c r="J57" s="79">
+        <v>2</v>
+      </c>
       <c r="K57" s="81"/>
-      <c r="L57" s="82"/>
+      <c r="L57" s="88" t="s">
+        <v>362</v>
+      </c>
       <c r="M57" s="78"/>
+      <c r="N57" s="1"/>
+      <c r="P57" s="3"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B58" s="77"/>
       <c r="C58" s="80">
-        <v>9</v>
-      </c>
-      <c r="D58" s="81"/>
-      <c r="E58" s="81"/>
+        <v>3</v>
+      </c>
+      <c r="D58" s="81" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" s="81" t="s">
+        <v>358</v>
+      </c>
       <c r="F58" s="79"/>
       <c r="G58" s="79"/>
-      <c r="H58" s="79"/>
-      <c r="I58" s="81"/>
-      <c r="J58" s="79"/>
+      <c r="H58" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="I58" s="88" t="s">
+        <v>962</v>
+      </c>
+      <c r="J58" s="79">
+        <v>10</v>
+      </c>
       <c r="K58" s="81"/>
-      <c r="L58" s="83"/>
+      <c r="L58" s="81"/>
       <c r="M58" s="78"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B59" s="77"/>
       <c r="C59" s="80">
-        <v>10</v>
-      </c>
-      <c r="D59" s="81"/>
-      <c r="E59" s="81"/>
+        <v>4</v>
+      </c>
+      <c r="D59" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="E59" s="81" t="s">
+        <v>359</v>
+      </c>
       <c r="F59" s="79"/>
       <c r="G59" s="79"/>
-      <c r="H59" s="79"/>
-      <c r="I59" s="81"/>
-      <c r="J59" s="79"/>
+      <c r="H59" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="I59" s="88" t="s">
+        <v>962</v>
+      </c>
+      <c r="J59" s="79">
+        <v>10</v>
+      </c>
       <c r="K59" s="81"/>
       <c r="L59" s="81"/>
       <c r="M59" s="78"/>
     </row>
-    <row r="60" spans="2:16" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B60" s="84"/>
-      <c r="C60" s="85"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="85"/>
-      <c r="F60" s="85"/>
-      <c r="G60" s="85"/>
-      <c r="H60" s="85"/>
-      <c r="I60" s="85"/>
-      <c r="J60" s="86"/>
-      <c r="K60" s="85"/>
-      <c r="L60" s="85"/>
-      <c r="M60" s="87"/>
-    </row>
-    <row r="61" spans="2:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="62" spans="2:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="73"/>
-      <c r="C62" s="74"/>
-      <c r="D62" s="74"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="74"/>
-      <c r="G62" s="74"/>
-      <c r="H62" s="74"/>
-      <c r="I62" s="74"/>
-      <c r="J62" s="75"/>
-      <c r="K62" s="74"/>
-      <c r="L62" s="74"/>
-      <c r="M62" s="76"/>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B60" s="77"/>
+      <c r="C60" s="80">
+        <v>5</v>
+      </c>
+      <c r="D60" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" s="81" t="s">
+        <v>343</v>
+      </c>
+      <c r="F60" s="79"/>
+      <c r="G60" s="79"/>
+      <c r="H60" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="I60" s="88" t="s">
+        <v>965</v>
+      </c>
+      <c r="J60" s="79"/>
+      <c r="K60" s="81"/>
+      <c r="L60" s="81"/>
+      <c r="M60" s="78"/>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B61" s="77"/>
+      <c r="C61" s="80">
+        <v>6</v>
+      </c>
+      <c r="D61" s="81" t="s">
+        <v>360</v>
+      </c>
+      <c r="E61" s="81" t="s">
+        <v>361</v>
+      </c>
+      <c r="F61" s="79"/>
+      <c r="G61" s="79"/>
+      <c r="H61" s="79" t="s">
+        <v>331</v>
+      </c>
+      <c r="I61" s="88" t="s">
+        <v>965</v>
+      </c>
+      <c r="J61" s="79"/>
+      <c r="K61" s="81"/>
+      <c r="L61" s="81"/>
+      <c r="M61" s="78"/>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B62" s="77"/>
+      <c r="C62" s="80">
+        <v>7</v>
+      </c>
+      <c r="D62" s="81"/>
+      <c r="E62" s="81"/>
+      <c r="F62" s="79"/>
+      <c r="G62" s="79"/>
+      <c r="H62" s="79"/>
+      <c r="I62" s="88"/>
+      <c r="J62" s="79"/>
+      <c r="K62" s="81"/>
+      <c r="L62" s="81"/>
+      <c r="M62" s="78"/>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B63" s="77"/>
-      <c r="C63" s="116" t="s">
-        <v>291</v>
-      </c>
-      <c r="D63" s="117"/>
-      <c r="E63" s="118" t="s">
-        <v>267</v>
-      </c>
-      <c r="F63" s="119"/>
-      <c r="G63" s="119"/>
-      <c r="H63" s="119"/>
-      <c r="I63" s="119"/>
-      <c r="J63" s="120"/>
-      <c r="K63" s="71"/>
-      <c r="L63" s="71"/>
+      <c r="C63" s="80">
+        <v>8</v>
+      </c>
+      <c r="D63" s="81"/>
+      <c r="E63" s="81"/>
+      <c r="F63" s="79"/>
+      <c r="G63" s="79"/>
+      <c r="H63" s="79"/>
+      <c r="I63" s="81"/>
+      <c r="J63" s="79"/>
+      <c r="K63" s="81"/>
+      <c r="L63" s="82"/>
       <c r="M63" s="78"/>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B64" s="77"/>
-      <c r="C64" s="116" t="s">
-        <v>292</v>
-      </c>
-      <c r="D64" s="117"/>
-      <c r="E64" s="118" t="s">
-        <v>365</v>
-      </c>
-      <c r="F64" s="119"/>
-      <c r="G64" s="119"/>
-      <c r="H64" s="119"/>
-      <c r="I64" s="119"/>
-      <c r="J64" s="120"/>
-      <c r="K64" s="71"/>
-      <c r="L64" s="71"/>
+      <c r="C64" s="80">
+        <v>9</v>
+      </c>
+      <c r="D64" s="81"/>
+      <c r="E64" s="81"/>
+      <c r="F64" s="79"/>
+      <c r="G64" s="79"/>
+      <c r="H64" s="79"/>
+      <c r="I64" s="81"/>
+      <c r="J64" s="79"/>
+      <c r="K64" s="81"/>
+      <c r="L64" s="83"/>
       <c r="M64" s="78"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B65" s="77"/>
-      <c r="C65" s="71"/>
-      <c r="D65" s="71"/>
-      <c r="E65" s="71"/>
-      <c r="F65" s="71"/>
-      <c r="G65" s="71"/>
-      <c r="H65" s="71"/>
-      <c r="I65" s="71"/>
-      <c r="J65" s="72"/>
-      <c r="K65" s="71"/>
-      <c r="L65" s="71"/>
+      <c r="C65" s="80">
+        <v>10</v>
+      </c>
+      <c r="D65" s="81"/>
+      <c r="E65" s="81"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="79"/>
+      <c r="H65" s="79"/>
+      <c r="I65" s="81"/>
+      <c r="J65" s="79"/>
+      <c r="K65" s="81"/>
+      <c r="L65" s="81"/>
       <c r="M65" s="78"/>
     </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B66" s="77"/>
-      <c r="C66" s="121" t="s">
-        <v>293</v>
-      </c>
-      <c r="D66" s="123" t="s">
-        <v>294</v>
-      </c>
-      <c r="E66" s="123"/>
-      <c r="F66" s="123" t="s">
-        <v>295</v>
-      </c>
-      <c r="G66" s="123"/>
-      <c r="H66" s="123"/>
-      <c r="I66" s="123" t="s">
-        <v>296</v>
-      </c>
-      <c r="J66" s="123"/>
-      <c r="K66" s="121" t="s">
-        <v>297</v>
-      </c>
-      <c r="L66" s="121" t="s">
-        <v>298</v>
-      </c>
-      <c r="M66" s="78"/>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B67" s="77"/>
-      <c r="C67" s="122"/>
-      <c r="D67" s="79" t="s">
-        <v>299</v>
-      </c>
-      <c r="E67" s="79" t="s">
-        <v>300</v>
-      </c>
-      <c r="F67" s="79" t="s">
-        <v>301</v>
-      </c>
-      <c r="G67" s="79" t="s">
-        <v>302</v>
-      </c>
-      <c r="H67" s="79" t="s">
-        <v>303</v>
-      </c>
-      <c r="I67" s="79" t="s">
-        <v>304</v>
-      </c>
-      <c r="J67" s="79" t="s">
-        <v>305</v>
-      </c>
-      <c r="K67" s="122"/>
-      <c r="L67" s="122"/>
-      <c r="M67" s="78"/>
+    <row r="66" spans="2:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B66" s="84"/>
+      <c r="C66" s="85"/>
+      <c r="D66" s="85"/>
+      <c r="E66" s="85"/>
+      <c r="F66" s="85"/>
+      <c r="G66" s="85"/>
+      <c r="H66" s="85"/>
+      <c r="I66" s="85"/>
+      <c r="J66" s="86"/>
+      <c r="K66" s="85"/>
+      <c r="L66" s="85"/>
+      <c r="M66" s="87"/>
+    </row>
+    <row r="67" spans="2:13" s="131" customFormat="1" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B67" s="129"/>
+      <c r="C67" s="129"/>
+      <c r="D67" s="129"/>
+      <c r="E67" s="129"/>
+      <c r="F67" s="129"/>
+      <c r="G67" s="129"/>
+      <c r="H67" s="129"/>
+      <c r="I67" s="129"/>
+      <c r="J67" s="130"/>
+      <c r="K67" s="129"/>
+      <c r="L67" s="129"/>
+      <c r="M67" s="129"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B68" s="77"/>
-      <c r="C68" s="80">
-        <v>1</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="E68" s="88" t="s">
-        <v>346</v>
-      </c>
-      <c r="F68" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="H68" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I68" s="81" t="s">
-        <v>340</v>
-      </c>
-      <c r="J68" s="79">
-        <v>3</v>
-      </c>
-      <c r="K68" s="81"/>
-      <c r="L68" s="81" t="s">
-        <v>351</v>
-      </c>
-      <c r="M68" s="78"/>
+      <c r="B68" s="73"/>
+      <c r="C68" s="74"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
+      <c r="F68" s="74"/>
+      <c r="G68" s="74"/>
+      <c r="H68" s="74"/>
+      <c r="I68" s="74"/>
+      <c r="J68" s="75"/>
+      <c r="K68" s="74"/>
+      <c r="L68" s="74"/>
+      <c r="M68" s="76"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B69" s="77"/>
-      <c r="C69" s="80">
-        <v>2</v>
-      </c>
-      <c r="D69" s="53" t="s">
-        <v>254</v>
-      </c>
-      <c r="E69" s="88" t="s">
-        <v>364</v>
-      </c>
-      <c r="F69" s="79"/>
-      <c r="G69" s="79"/>
-      <c r="H69" s="79" t="s">
-        <v>331</v>
-      </c>
-      <c r="I69" s="88" t="s">
-        <v>335</v>
-      </c>
-      <c r="J69" s="79">
-        <v>10</v>
-      </c>
-      <c r="K69" s="81"/>
-      <c r="L69" s="81"/>
+      <c r="C69" s="123" t="s">
+        <v>291</v>
+      </c>
+      <c r="D69" s="124"/>
+      <c r="E69" s="125" t="s">
+        <v>265</v>
+      </c>
+      <c r="F69" s="126"/>
+      <c r="G69" s="126"/>
+      <c r="H69" s="126"/>
+      <c r="I69" s="126"/>
+      <c r="J69" s="127"/>
+      <c r="K69" s="129"/>
+      <c r="L69" s="129"/>
       <c r="M69" s="78"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B70" s="77"/>
-      <c r="C70" s="80">
-        <v>3</v>
-      </c>
-      <c r="D70" s="81"/>
-      <c r="E70" s="81"/>
-      <c r="F70" s="79"/>
-      <c r="G70" s="79"/>
-      <c r="H70" s="79"/>
-      <c r="I70" s="81"/>
-      <c r="J70" s="79"/>
-      <c r="K70" s="81"/>
-      <c r="L70" s="81"/>
+      <c r="C70" s="123" t="s">
+        <v>292</v>
+      </c>
+      <c r="D70" s="124"/>
+      <c r="E70" s="125" t="s">
+        <v>353</v>
+      </c>
+      <c r="F70" s="126"/>
+      <c r="G70" s="126"/>
+      <c r="H70" s="126"/>
+      <c r="I70" s="126"/>
+      <c r="J70" s="127"/>
+      <c r="K70" s="129"/>
+      <c r="L70" s="129"/>
       <c r="M70" s="78"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B71" s="77"/>
-      <c r="C71" s="80">
-        <v>4</v>
-      </c>
-      <c r="D71" s="81"/>
-      <c r="E71" s="81"/>
-      <c r="F71" s="79"/>
-      <c r="G71" s="79"/>
-      <c r="H71" s="79"/>
-      <c r="I71" s="81"/>
-      <c r="J71" s="79"/>
-      <c r="K71" s="81"/>
-      <c r="L71" s="81"/>
+      <c r="C71" s="129"/>
+      <c r="D71" s="129"/>
+      <c r="E71" s="129"/>
+      <c r="F71" s="129"/>
+      <c r="G71" s="129"/>
+      <c r="H71" s="129"/>
+      <c r="I71" s="129"/>
+      <c r="J71" s="130"/>
+      <c r="K71" s="129"/>
+      <c r="L71" s="129"/>
       <c r="M71" s="78"/>
     </row>
-    <row r="72" spans="2:13" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B72" s="84"/>
-      <c r="C72" s="85"/>
-      <c r="D72" s="85"/>
-      <c r="E72" s="85"/>
-      <c r="F72" s="85"/>
-      <c r="G72" s="85"/>
-      <c r="H72" s="85"/>
-      <c r="I72" s="85"/>
-      <c r="J72" s="86"/>
-      <c r="K72" s="85"/>
-      <c r="L72" s="85"/>
-      <c r="M72" s="87"/>
-    </row>
-    <row r="73" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="74" spans="2:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B74" s="73"/>
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-      <c r="F74" s="74"/>
-      <c r="G74" s="74"/>
-      <c r="H74" s="74"/>
-      <c r="I74" s="74"/>
-      <c r="J74" s="75"/>
-      <c r="K74" s="74"/>
-      <c r="L74" s="74"/>
-      <c r="M74" s="76"/>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B72" s="77"/>
+      <c r="C72" s="121" t="s">
+        <v>293</v>
+      </c>
+      <c r="D72" s="128" t="s">
+        <v>294</v>
+      </c>
+      <c r="E72" s="128"/>
+      <c r="F72" s="128" t="s">
+        <v>295</v>
+      </c>
+      <c r="G72" s="128"/>
+      <c r="H72" s="128"/>
+      <c r="I72" s="128" t="s">
+        <v>296</v>
+      </c>
+      <c r="J72" s="128"/>
+      <c r="K72" s="121" t="s">
+        <v>297</v>
+      </c>
+      <c r="L72" s="121" t="s">
+        <v>298</v>
+      </c>
+      <c r="M72" s="78"/>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B73" s="77"/>
+      <c r="C73" s="122"/>
+      <c r="D73" s="114" t="s">
+        <v>299</v>
+      </c>
+      <c r="E73" s="114" t="s">
+        <v>300</v>
+      </c>
+      <c r="F73" s="114" t="s">
+        <v>301</v>
+      </c>
+      <c r="G73" s="114" t="s">
+        <v>302</v>
+      </c>
+      <c r="H73" s="114" t="s">
+        <v>303</v>
+      </c>
+      <c r="I73" s="114" t="s">
+        <v>304</v>
+      </c>
+      <c r="J73" s="114" t="s">
+        <v>305</v>
+      </c>
+      <c r="K73" s="122"/>
+      <c r="L73" s="122"/>
+      <c r="M73" s="78"/>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B74" s="77"/>
+      <c r="C74" s="80">
+        <v>1</v>
+      </c>
+      <c r="D74" s="81" t="s">
+        <v>264</v>
+      </c>
+      <c r="E74" s="88" t="s">
+        <v>345</v>
+      </c>
+      <c r="F74" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="G74" s="114"/>
+      <c r="H74" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I74" s="88" t="s">
+        <v>333</v>
+      </c>
+      <c r="J74" s="114"/>
+      <c r="K74" s="81"/>
+      <c r="L74" s="89" t="s">
+        <v>350</v>
+      </c>
+      <c r="M74" s="78"/>
     </row>
     <row r="75" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B75" s="77"/>
-      <c r="C75" s="116" t="s">
-        <v>291</v>
-      </c>
-      <c r="D75" s="117"/>
-      <c r="E75" s="118" t="s">
-        <v>250</v>
-      </c>
-      <c r="F75" s="119"/>
-      <c r="G75" s="119"/>
-      <c r="H75" s="119"/>
-      <c r="I75" s="119"/>
-      <c r="J75" s="120"/>
-      <c r="K75" s="71"/>
-      <c r="L75" s="71"/>
+      <c r="C75" s="80">
+        <v>2</v>
+      </c>
+      <c r="D75" s="81" t="s">
+        <v>282</v>
+      </c>
+      <c r="E75" s="81" t="s">
+        <v>342</v>
+      </c>
+      <c r="F75" s="114"/>
+      <c r="G75" s="114"/>
+      <c r="H75" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I75" s="88" t="s">
+        <v>307</v>
+      </c>
+      <c r="J75" s="114"/>
+      <c r="K75" s="81"/>
+      <c r="L75" s="81"/>
       <c r="M75" s="78"/>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B76" s="77"/>
-      <c r="C76" s="116" t="s">
-        <v>292</v>
-      </c>
-      <c r="D76" s="117"/>
-      <c r="E76" s="118" t="s">
-        <v>963</v>
-      </c>
-      <c r="F76" s="119"/>
-      <c r="G76" s="119"/>
-      <c r="H76" s="119"/>
-      <c r="I76" s="119"/>
-      <c r="J76" s="120"/>
-      <c r="K76" s="71"/>
-      <c r="L76" s="71"/>
+      <c r="C76" s="80">
+        <v>3</v>
+      </c>
+      <c r="D76" s="81" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="88" t="s">
+        <v>318</v>
+      </c>
+      <c r="F76" s="114"/>
+      <c r="G76" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="H76" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I76" s="88" t="s">
+        <v>306</v>
+      </c>
+      <c r="J76" s="114">
+        <v>5</v>
+      </c>
+      <c r="K76" s="81"/>
+      <c r="L76" s="88" t="s">
+        <v>352</v>
+      </c>
       <c r="M76" s="78"/>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B77" s="77"/>
-      <c r="C77" s="71"/>
-      <c r="D77" s="71"/>
-      <c r="E77" s="71"/>
-      <c r="F77" s="71"/>
-      <c r="G77" s="71"/>
-      <c r="H77" s="71"/>
-      <c r="I77" s="71"/>
-      <c r="J77" s="72"/>
-      <c r="K77" s="71"/>
-      <c r="L77" s="71"/>
+      <c r="C77" s="80">
+        <v>4</v>
+      </c>
+      <c r="D77" s="88" t="s">
+        <v>262</v>
+      </c>
+      <c r="E77" s="88" t="s">
+        <v>356</v>
+      </c>
+      <c r="F77" s="114"/>
+      <c r="G77" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="H77" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I77" s="88" t="s">
+        <v>306</v>
+      </c>
+      <c r="J77" s="114">
+        <v>5</v>
+      </c>
+      <c r="K77" s="81"/>
+      <c r="L77" s="88" t="s">
+        <v>363</v>
+      </c>
       <c r="M77" s="78"/>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B78" s="77"/>
-      <c r="C78" s="121" t="s">
-        <v>293</v>
-      </c>
-      <c r="D78" s="123" t="s">
-        <v>294</v>
-      </c>
-      <c r="E78" s="123"/>
-      <c r="F78" s="123" t="s">
-        <v>295</v>
-      </c>
-      <c r="G78" s="123"/>
-      <c r="H78" s="123"/>
-      <c r="I78" s="123" t="s">
-        <v>296</v>
-      </c>
-      <c r="J78" s="123"/>
-      <c r="K78" s="121" t="s">
-        <v>297</v>
-      </c>
-      <c r="L78" s="121" t="s">
-        <v>298</v>
-      </c>
+      <c r="C78" s="80">
+        <v>5</v>
+      </c>
+      <c r="D78" s="88" t="s">
+        <v>309</v>
+      </c>
+      <c r="E78" s="81" t="s">
+        <v>343</v>
+      </c>
+      <c r="F78" s="114"/>
+      <c r="G78" s="131"/>
+      <c r="H78" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I78" s="88" t="s">
+        <v>333</v>
+      </c>
+      <c r="J78" s="114"/>
+      <c r="K78" s="81"/>
+      <c r="L78" s="81"/>
       <c r="M78" s="78"/>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B79" s="77"/>
-      <c r="C79" s="122"/>
-      <c r="D79" s="111" t="s">
-        <v>299</v>
-      </c>
-      <c r="E79" s="111" t="s">
-        <v>300</v>
-      </c>
-      <c r="F79" s="111" t="s">
-        <v>301</v>
-      </c>
-      <c r="G79" s="111" t="s">
-        <v>302</v>
-      </c>
-      <c r="H79" s="111" t="s">
-        <v>303</v>
-      </c>
-      <c r="I79" s="111" t="s">
-        <v>304</v>
-      </c>
-      <c r="J79" s="111" t="s">
-        <v>305</v>
-      </c>
-      <c r="K79" s="122"/>
-      <c r="L79" s="122"/>
+      <c r="C79" s="80">
+        <v>6</v>
+      </c>
+      <c r="D79" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="E79" s="81" t="s">
+        <v>344</v>
+      </c>
+      <c r="F79" s="114"/>
+      <c r="G79" s="114"/>
+      <c r="H79" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I79" s="88" t="s">
+        <v>333</v>
+      </c>
+      <c r="J79" s="114"/>
+      <c r="K79" s="81"/>
+      <c r="L79" s="81"/>
       <c r="M79" s="78"/>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B80" s="77"/>
       <c r="C80" s="80">
-        <v>1</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>959</v>
+        <v>7</v>
+      </c>
+      <c r="D80" s="81" t="s">
+        <v>268</v>
       </c>
       <c r="E80" s="88" t="s">
-        <v>964</v>
-      </c>
-      <c r="F80" s="111" t="s">
-        <v>331</v>
-      </c>
-      <c r="H80" s="111" t="s">
-        <v>331</v>
-      </c>
-      <c r="I80" s="81" t="s">
-        <v>340</v>
-      </c>
-      <c r="J80" s="111">
-        <v>2</v>
+        <v>346</v>
+      </c>
+      <c r="F80" s="114"/>
+      <c r="G80" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="H80" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="I80" s="88" t="s">
+        <v>306</v>
+      </c>
+      <c r="J80" s="114">
+        <v>3</v>
       </c>
       <c r="K80" s="81"/>
-      <c r="L80" s="81" t="s">
-        <v>362</v>
+      <c r="L80" s="88" t="s">
+        <v>351</v>
       </c>
       <c r="M80" s="78"/>
     </row>
     <row r="81" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B81" s="77"/>
       <c r="C81" s="80">
-        <v>2</v>
-      </c>
-      <c r="D81" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="E81" s="88" t="s">
-        <v>357</v>
-      </c>
-      <c r="F81" s="111"/>
-      <c r="G81" s="111"/>
-      <c r="H81" s="111" t="s">
-        <v>331</v>
-      </c>
-      <c r="I81" s="88" t="s">
-        <v>962</v>
-      </c>
-      <c r="J81" s="111">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D81" s="88"/>
+      <c r="E81" s="81"/>
+      <c r="F81" s="114"/>
+      <c r="G81" s="131"/>
+      <c r="H81" s="114"/>
+      <c r="I81" s="81"/>
+      <c r="J81" s="114"/>
       <c r="K81" s="81"/>
-      <c r="L81" s="81"/>
+      <c r="L81" s="82"/>
       <c r="M81" s="78"/>
     </row>
     <row r="82" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B82" s="77"/>
       <c r="C82" s="80">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D82" s="81"/>
       <c r="E82" s="81"/>
-      <c r="F82" s="111"/>
-      <c r="G82" s="111"/>
-      <c r="H82" s="111"/>
+      <c r="F82" s="114"/>
+      <c r="G82" s="114"/>
+      <c r="H82" s="114"/>
       <c r="I82" s="81"/>
-      <c r="J82" s="111"/>
+      <c r="J82" s="114"/>
       <c r="K82" s="81"/>
-      <c r="L82" s="81"/>
+      <c r="L82" s="83"/>
       <c r="M82" s="78"/>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B83" s="77"/>
       <c r="C83" s="80">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D83" s="81"/>
       <c r="E83" s="81"/>
-      <c r="F83" s="111"/>
-      <c r="G83" s="111"/>
-      <c r="H83" s="111"/>
+      <c r="F83" s="114"/>
+      <c r="G83" s="114"/>
+      <c r="H83" s="114"/>
       <c r="I83" s="81"/>
-      <c r="J83" s="111"/>
+      <c r="J83" s="114"/>
       <c r="K83" s="81"/>
       <c r="L83" s="81"/>
       <c r="M83" s="78"/>
     </row>
-    <row r="84" spans="2:13" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:13" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B84" s="84"/>
       <c r="C84" s="85"/>
       <c r="D84" s="85"/>
@@ -9182,39 +9221,37 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="K78:K79"/>
-    <mergeCell ref="L78:L79"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E75:J75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="E76:J76"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="I78:J78"/>
-    <mergeCell ref="L66:L67"/>
-    <mergeCell ref="K48:K49"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E63:J63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:J64"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="K66:K67"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:J45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:J46"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="L72:L73"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="E69:J69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E70:J70"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="K72:K73"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:J51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:J52"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="K54:K55"/>
+    <mergeCell ref="L54:L55"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:J27"/>
     <mergeCell ref="C28:D28"/>
@@ -9224,14 +9261,16 @@
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="K30:K31"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="L42:L43"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="I42:J42"/>
   </mergeCells>
   <phoneticPr fontId="8"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9243,8 +9282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2AA5EF-E9D7-46ED-AD7B-B086BE7AB8F6}">
   <dimension ref="B2:AH86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -9436,7 +9475,7 @@
       <c r="P4" s="13">
         <v>1</v>
       </c>
-      <c r="Q4" s="127">
+      <c r="Q4" s="118">
         <v>45575</v>
       </c>
       <c r="R4" s="13">
@@ -9469,7 +9508,7 @@
       <c r="AB4" s="13">
         <v>1540</v>
       </c>
-      <c r="AD4" s="126" t="s">
+      <c r="AD4" s="117" t="s">
         <v>1046</v>
       </c>
       <c r="AE4" s="13" t="s">
@@ -9525,7 +9564,7 @@
       <c r="P5" s="13">
         <v>2</v>
       </c>
-      <c r="Q5" s="127">
+      <c r="Q5" s="118">
         <v>45576</v>
       </c>
       <c r="R5" s="13">
@@ -9558,7 +9597,7 @@
       <c r="AB5" s="13">
         <v>1200</v>
       </c>
-      <c r="AD5" s="126" t="s">
+      <c r="AD5" s="117" t="s">
         <v>1047</v>
       </c>
       <c r="AE5" s="13" t="s">
@@ -9614,7 +9653,7 @@
       <c r="P6" s="13">
         <v>3</v>
       </c>
-      <c r="Q6" s="127">
+      <c r="Q6" s="118">
         <v>45577</v>
       </c>
       <c r="R6" s="13">
@@ -9647,7 +9686,7 @@
       <c r="AB6" s="13">
         <v>1300</v>
       </c>
-      <c r="AD6" s="126" t="s">
+      <c r="AD6" s="117" t="s">
         <v>1048</v>
       </c>
       <c r="AE6" s="13" t="s">
@@ -9703,7 +9742,7 @@
       <c r="P7" s="13">
         <v>4</v>
       </c>
-      <c r="Q7" s="127">
+      <c r="Q7" s="118">
         <v>45578</v>
       </c>
       <c r="R7" s="13">
@@ -9736,7 +9775,7 @@
       <c r="AB7" s="13">
         <v>900</v>
       </c>
-      <c r="AD7" s="125"/>
+      <c r="AD7" s="116"/>
       <c r="AG7" s="13">
         <v>15</v>
       </c>
@@ -9787,7 +9826,7 @@
       <c r="P8" s="13">
         <v>5</v>
       </c>
-      <c r="Q8" s="127">
+      <c r="Q8" s="118">
         <v>45579</v>
       </c>
       <c r="R8" s="13">
@@ -9820,7 +9859,7 @@
       <c r="AB8" s="13">
         <v>400</v>
       </c>
-      <c r="AD8" s="125"/>
+      <c r="AD8" s="116"/>
       <c r="AG8" s="13">
         <v>20</v>
       </c>
@@ -9871,7 +9910,7 @@
       <c r="P9" s="13">
         <v>6</v>
       </c>
-      <c r="Q9" s="127">
+      <c r="Q9" s="118">
         <v>45580</v>
       </c>
       <c r="R9" s="13">
@@ -9904,7 +9943,7 @@
       <c r="AB9" s="13">
         <v>500</v>
       </c>
-      <c r="AD9" s="125"/>
+      <c r="AD9" s="116"/>
       <c r="AG9" s="13">
         <v>21</v>
       </c>
@@ -9955,7 +9994,7 @@
       <c r="P10" s="13">
         <v>7</v>
       </c>
-      <c r="Q10" s="127">
+      <c r="Q10" s="118">
         <v>45581</v>
       </c>
       <c r="R10" s="13">
@@ -9988,7 +10027,7 @@
       <c r="AB10" s="13">
         <v>2500</v>
       </c>
-      <c r="AD10" s="125"/>
+      <c r="AD10" s="116"/>
       <c r="AG10" s="13">
         <v>22</v>
       </c>
@@ -10039,7 +10078,7 @@
       <c r="P11" s="13">
         <v>8</v>
       </c>
-      <c r="Q11" s="127">
+      <c r="Q11" s="118">
         <v>45582</v>
       </c>
       <c r="R11" s="13">
@@ -10072,7 +10111,7 @@
       <c r="AB11" s="13">
         <v>300</v>
       </c>
-      <c r="AD11" s="125"/>
+      <c r="AD11" s="116"/>
     </row>
     <row r="12" spans="2:34" x14ac:dyDescent="0.4">
       <c r="B12" s="100" t="s">
@@ -10117,7 +10156,7 @@
       <c r="P12" s="13">
         <v>9</v>
       </c>
-      <c r="Q12" s="127">
+      <c r="Q12" s="118">
         <v>45583</v>
       </c>
       <c r="R12" s="13">
@@ -10150,7 +10189,7 @@
       <c r="AB12" s="13">
         <v>1100</v>
       </c>
-      <c r="AD12" s="125"/>
+      <c r="AD12" s="116"/>
     </row>
     <row r="13" spans="2:34" x14ac:dyDescent="0.4">
       <c r="B13" s="100" t="s">
@@ -10195,7 +10234,7 @@
       <c r="P13" s="13">
         <v>10</v>
       </c>
-      <c r="Q13" s="127">
+      <c r="Q13" s="118">
         <v>45584</v>
       </c>
       <c r="R13" s="13">
@@ -10228,7 +10267,7 @@
       <c r="AB13" s="13">
         <v>150</v>
       </c>
-      <c r="AD13" s="125"/>
+      <c r="AD13" s="116"/>
     </row>
     <row r="14" spans="2:34" x14ac:dyDescent="0.4">
       <c r="B14" s="100" t="s">
@@ -10273,7 +10312,7 @@
       <c r="P14" s="13">
         <v>11</v>
       </c>
-      <c r="Q14" s="127">
+      <c r="Q14" s="118">
         <v>45585</v>
       </c>
       <c r="R14" s="13">
@@ -10306,7 +10345,7 @@
       <c r="AB14" s="13">
         <v>1800</v>
       </c>
-      <c r="AD14" s="125"/>
+      <c r="AD14" s="116"/>
     </row>
     <row r="15" spans="2:34" x14ac:dyDescent="0.4">
       <c r="B15" s="100" t="s">
@@ -10351,7 +10390,7 @@
       <c r="P15" s="13">
         <v>12</v>
       </c>
-      <c r="Q15" s="127">
+      <c r="Q15" s="118">
         <v>45586</v>
       </c>
       <c r="R15" s="13">
@@ -10384,7 +10423,7 @@
       <c r="AB15" s="13">
         <v>2000</v>
       </c>
-      <c r="AD15" s="125"/>
+      <c r="AD15" s="116"/>
     </row>
     <row r="16" spans="2:34" x14ac:dyDescent="0.4">
       <c r="B16" s="100" t="s">
@@ -10429,7 +10468,7 @@
       <c r="P16" s="13">
         <v>13</v>
       </c>
-      <c r="Q16" s="127">
+      <c r="Q16" s="118">
         <v>45587</v>
       </c>
       <c r="R16" s="13">
@@ -10462,7 +10501,7 @@
       <c r="AB16" s="13">
         <v>1500</v>
       </c>
-      <c r="AD16" s="125"/>
+      <c r="AD16" s="116"/>
     </row>
     <row r="17" spans="2:30" x14ac:dyDescent="0.4">
       <c r="B17" s="100" t="s">
@@ -10507,7 +10546,7 @@
       <c r="P17" s="13">
         <v>14</v>
       </c>
-      <c r="Q17" s="127">
+      <c r="Q17" s="118">
         <v>45588</v>
       </c>
       <c r="R17" s="13">
@@ -10540,7 +10579,7 @@
       <c r="AB17" s="13">
         <v>600</v>
       </c>
-      <c r="AD17" s="125"/>
+      <c r="AD17" s="116"/>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.4">
       <c r="B18" s="100" t="s">
@@ -10585,7 +10624,7 @@
       <c r="P18" s="13">
         <v>15</v>
       </c>
-      <c r="Q18" s="127">
+      <c r="Q18" s="118">
         <v>45589</v>
       </c>
       <c r="R18" s="13">
@@ -10618,7 +10657,7 @@
       <c r="AB18" s="13">
         <v>450</v>
       </c>
-      <c r="AD18" s="125"/>
+      <c r="AD18" s="116"/>
     </row>
     <row r="19" spans="2:30" x14ac:dyDescent="0.4">
       <c r="B19" s="100" t="s">
@@ -10663,7 +10702,7 @@
       <c r="P19" s="13">
         <v>16</v>
       </c>
-      <c r="Q19" s="127">
+      <c r="Q19" s="118">
         <v>45590</v>
       </c>
       <c r="R19" s="13">
@@ -10696,7 +10735,7 @@
       <c r="AB19" s="13">
         <v>550</v>
       </c>
-      <c r="AD19" s="125"/>
+      <c r="AD19" s="116"/>
     </row>
     <row r="20" spans="2:30" x14ac:dyDescent="0.4">
       <c r="B20" s="100" t="s">
@@ -10741,7 +10780,7 @@
       <c r="P20" s="13">
         <v>17</v>
       </c>
-      <c r="Q20" s="127">
+      <c r="Q20" s="118">
         <v>45591</v>
       </c>
       <c r="R20" s="13">
@@ -10774,7 +10813,7 @@
       <c r="AB20" s="13">
         <v>2800</v>
       </c>
-      <c r="AD20" s="125"/>
+      <c r="AD20" s="116"/>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.4">
       <c r="B21" s="100" t="s">
@@ -10819,7 +10858,7 @@
       <c r="P21" s="13">
         <v>18</v>
       </c>
-      <c r="Q21" s="127">
+      <c r="Q21" s="118">
         <v>45592</v>
       </c>
       <c r="R21" s="13">
@@ -10852,7 +10891,7 @@
       <c r="AB21" s="13">
         <v>350</v>
       </c>
-      <c r="AD21" s="125"/>
+      <c r="AD21" s="116"/>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.4">
       <c r="B22" s="100" t="s">
@@ -10897,7 +10936,7 @@
       <c r="P22" s="13">
         <v>19</v>
       </c>
-      <c r="Q22" s="127">
+      <c r="Q22" s="118">
         <v>45593</v>
       </c>
       <c r="R22" s="13">
@@ -10930,7 +10969,7 @@
       <c r="AB22" s="13">
         <v>750</v>
       </c>
-      <c r="AD22" s="125"/>
+      <c r="AD22" s="116"/>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.4">
       <c r="B23" s="100" t="s">
@@ -10975,7 +11014,7 @@
       <c r="P23" s="13">
         <v>20</v>
       </c>
-      <c r="Q23" s="127">
+      <c r="Q23" s="118">
         <v>45594</v>
       </c>
       <c r="R23" s="13">
@@ -11008,7 +11047,7 @@
       <c r="AB23" s="13">
         <v>850</v>
       </c>
-      <c r="AD23" s="125"/>
+      <c r="AD23" s="116"/>
     </row>
     <row r="24" spans="2:30" x14ac:dyDescent="0.4">
       <c r="B24" s="100" t="s">
@@ -11053,7 +11092,7 @@
       <c r="P24" s="13">
         <v>21</v>
       </c>
-      <c r="Q24" s="127">
+      <c r="Q24" s="118">
         <v>45595</v>
       </c>
       <c r="R24" s="13">
@@ -11130,7 +11169,7 @@
       <c r="P25" s="13">
         <v>22</v>
       </c>
-      <c r="Q25" s="127">
+      <c r="Q25" s="118">
         <v>45596</v>
       </c>
       <c r="R25" s="13">
@@ -11207,7 +11246,7 @@
       <c r="P26" s="13">
         <v>23</v>
       </c>
-      <c r="Q26" s="127">
+      <c r="Q26" s="118">
         <v>45597</v>
       </c>
       <c r="R26" s="13">
@@ -11284,7 +11323,7 @@
       <c r="P27" s="13">
         <v>24</v>
       </c>
-      <c r="Q27" s="127">
+      <c r="Q27" s="118">
         <v>45598</v>
       </c>
       <c r="R27" s="13">
@@ -11361,7 +11400,7 @@
       <c r="P28" s="13">
         <v>25</v>
       </c>
-      <c r="Q28" s="127">
+      <c r="Q28" s="118">
         <v>45599</v>
       </c>
       <c r="R28" s="13">
@@ -11438,7 +11477,7 @@
       <c r="P29" s="13">
         <v>26</v>
       </c>
-      <c r="Q29" s="127">
+      <c r="Q29" s="118">
         <v>45600</v>
       </c>
       <c r="R29" s="13">
@@ -11515,7 +11554,7 @@
       <c r="P30" s="13">
         <v>27</v>
       </c>
-      <c r="Q30" s="127">
+      <c r="Q30" s="118">
         <v>45601</v>
       </c>
       <c r="R30" s="13">
@@ -11592,7 +11631,7 @@
       <c r="P31" s="13">
         <v>28</v>
       </c>
-      <c r="Q31" s="127">
+      <c r="Q31" s="118">
         <v>45602</v>
       </c>
       <c r="R31" s="13">
@@ -11669,7 +11708,7 @@
       <c r="P32" s="13">
         <v>29</v>
       </c>
-      <c r="Q32" s="127">
+      <c r="Q32" s="118">
         <v>45603</v>
       </c>
       <c r="R32" s="13">
@@ -11746,7 +11785,7 @@
       <c r="P33" s="13">
         <v>30</v>
       </c>
-      <c r="Q33" s="127">
+      <c r="Q33" s="118">
         <v>45604</v>
       </c>
       <c r="R33" s="13">
@@ -11902,7 +11941,7 @@
       <c r="N36" s="109" t="s">
         <v>692</v>
       </c>
-      <c r="Q36" s="124"/>
+      <c r="Q36" s="115"/>
     </row>
     <row r="37" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B37" s="95" t="s">
@@ -11944,7 +11983,7 @@
       <c r="N37" s="109" t="s">
         <v>701</v>
       </c>
-      <c r="Q37" s="124"/>
+      <c r="Q37" s="115"/>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B38" s="95" t="s">
@@ -11986,7 +12025,7 @@
       <c r="N38" s="109" t="s">
         <v>711</v>
       </c>
-      <c r="Q38" s="124"/>
+      <c r="Q38" s="115"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B39" s="95" t="s">
@@ -12028,7 +12067,7 @@
       <c r="N39" s="109" t="s">
         <v>722</v>
       </c>
-      <c r="Q39" s="124"/>
+      <c r="Q39" s="115"/>
     </row>
     <row r="40" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B40" s="95" t="s">
@@ -12070,7 +12109,7 @@
       <c r="N40" s="109" t="s">
         <v>732</v>
       </c>
-      <c r="Q40" s="124"/>
+      <c r="Q40" s="115"/>
     </row>
     <row r="41" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B41" s="95" t="s">
@@ -12112,7 +12151,7 @@
       <c r="N41" s="109" t="s">
         <v>741</v>
       </c>
-      <c r="Q41" s="124"/>
+      <c r="Q41" s="115"/>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B42" s="95" t="s">
@@ -12154,7 +12193,7 @@
       <c r="N42" s="109" t="s">
         <v>749</v>
       </c>
-      <c r="Q42" s="124"/>
+      <c r="Q42" s="115"/>
     </row>
     <row r="43" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B43" s="95" t="s">
@@ -12196,7 +12235,7 @@
       <c r="N43" s="109" t="s">
         <v>758</v>
       </c>
-      <c r="Q43" s="124"/>
+      <c r="Q43" s="115"/>
     </row>
     <row r="44" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B44" s="95" t="s">
@@ -12238,7 +12277,7 @@
       <c r="N44" s="109" t="s">
         <v>761</v>
       </c>
-      <c r="Q44" s="124"/>
+      <c r="Q44" s="115"/>
     </row>
     <row r="45" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B45" s="95" t="s">
@@ -12280,7 +12319,7 @@
       <c r="N45" s="109" t="s">
         <v>764</v>
       </c>
-      <c r="Q45" s="124"/>
+      <c r="Q45" s="115"/>
     </row>
     <row r="46" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B46" s="95" t="s">
@@ -12322,7 +12361,7 @@
       <c r="N46" s="109" t="s">
         <v>767</v>
       </c>
-      <c r="Q46" s="124"/>
+      <c r="Q46" s="115"/>
     </row>
     <row r="47" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B47" s="95" t="s">
@@ -12364,7 +12403,7 @@
       <c r="N47" s="109" t="s">
         <v>770</v>
       </c>
-      <c r="Q47" s="124"/>
+      <c r="Q47" s="115"/>
     </row>
     <row r="48" spans="2:28" x14ac:dyDescent="0.4">
       <c r="B48" s="95" t="s">
@@ -12406,7 +12445,7 @@
       <c r="N48" s="109" t="s">
         <v>773</v>
       </c>
-      <c r="Q48" s="124"/>
+      <c r="Q48" s="115"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B49" s="95" t="s">
@@ -12448,7 +12487,7 @@
       <c r="N49" s="109" t="s">
         <v>776</v>
       </c>
-      <c r="Q49" s="124"/>
+      <c r="Q49" s="115"/>
     </row>
     <row r="50" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B50" s="95" t="s">
@@ -12490,7 +12529,7 @@
       <c r="N50" s="109" t="s">
         <v>779</v>
       </c>
-      <c r="Q50" s="124"/>
+      <c r="Q50" s="115"/>
     </row>
     <row r="51" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B51" s="95" t="s">
@@ -12532,7 +12571,7 @@
       <c r="N51" s="109" t="s">
         <v>782</v>
       </c>
-      <c r="Q51" s="124"/>
+      <c r="Q51" s="115"/>
     </row>
     <row r="52" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B52" s="95" t="s">
@@ -12574,7 +12613,7 @@
       <c r="N52" s="109" t="s">
         <v>785</v>
       </c>
-      <c r="Q52" s="124"/>
+      <c r="Q52" s="115"/>
     </row>
     <row r="53" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B53" s="95" t="s">
@@ -12616,7 +12655,7 @@
       <c r="N53" s="109" t="s">
         <v>788</v>
       </c>
-      <c r="Q53" s="124"/>
+      <c r="Q53" s="115"/>
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B54" s="95" t="s">
@@ -12658,7 +12697,7 @@
       <c r="N54" s="109" t="s">
         <v>791</v>
       </c>
-      <c r="Q54" s="124"/>
+      <c r="Q54" s="115"/>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B55" s="95" t="s">
@@ -12700,7 +12739,7 @@
       <c r="N55" s="109" t="s">
         <v>794</v>
       </c>
-      <c r="Q55" s="124"/>
+      <c r="Q55" s="115"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B56" s="95" t="s">
@@ -12742,7 +12781,7 @@
       <c r="N56" s="109" t="s">
         <v>797</v>
       </c>
-      <c r="Q56" s="124"/>
+      <c r="Q56" s="115"/>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B57" s="95" t="s">
@@ -12784,7 +12823,7 @@
       <c r="N57" s="109" t="s">
         <v>800</v>
       </c>
-      <c r="Q57" s="124"/>
+      <c r="Q57" s="115"/>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B58" s="95" t="s">
@@ -12826,7 +12865,7 @@
       <c r="N58" s="109" t="s">
         <v>803</v>
       </c>
-      <c r="Q58" s="124"/>
+      <c r="Q58" s="115"/>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B59" s="95" t="s">
@@ -12868,7 +12907,7 @@
       <c r="N59" s="109" t="s">
         <v>806</v>
       </c>
-      <c r="Q59" s="124"/>
+      <c r="Q59" s="115"/>
     </row>
     <row r="60" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B60" s="95" t="s">
@@ -12910,7 +12949,7 @@
       <c r="N60" s="109" t="s">
         <v>809</v>
       </c>
-      <c r="Q60" s="124"/>
+      <c r="Q60" s="115"/>
     </row>
     <row r="61" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B61" s="95" t="s">
@@ -12952,7 +12991,7 @@
       <c r="N61" s="109" t="s">
         <v>812</v>
       </c>
-      <c r="Q61" s="124"/>
+      <c r="Q61" s="115"/>
     </row>
     <row r="62" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B62" s="95" t="s">
@@ -12994,7 +13033,7 @@
       <c r="N62" s="109" t="s">
         <v>815</v>
       </c>
-      <c r="Q62" s="124"/>
+      <c r="Q62" s="115"/>
     </row>
     <row r="63" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B63" s="95" t="s">
@@ -13036,7 +13075,7 @@
       <c r="N63" s="109" t="s">
         <v>818</v>
       </c>
-      <c r="Q63" s="124"/>
+      <c r="Q63" s="115"/>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B64" s="95" t="s">
@@ -13078,7 +13117,7 @@
       <c r="N64" s="109" t="s">
         <v>821</v>
       </c>
-      <c r="Q64" s="124"/>
+      <c r="Q64" s="115"/>
     </row>
     <row r="65" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B65" s="95" t="s">
@@ -13120,7 +13159,7 @@
       <c r="N65" s="109" t="s">
         <v>824</v>
       </c>
-      <c r="Q65" s="124"/>
+      <c r="Q65" s="115"/>
     </row>
     <row r="66" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B66" s="95" t="s">
@@ -16621,14 +16660,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="39"/>
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="119" t="s">
         <v>322</v>
       </c>
-      <c r="C8" s="115"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="115"/>
-      <c r="G8" s="115"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="39"/>

</xml_diff>